<commit_message>
there was a -1 count that I changed to 1 in the Chinook
</commit_message>
<xml_diff>
--- a/Data/Ballard Locks Fish Counts/BallardLocksFinal2017 - daily.xlsx
+++ b/Data/Ballard Locks Fish Counts/BallardLocksFinal2017 - daily.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Allyn\Documents\GitHub\PinnipedCaseStudies\Data\Ballard Locks Fish Counts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB98EF09-0EF3-498A-A964-0DF307727BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="2160" yWindow="720" windowWidth="24960" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
     <sheet name="Historical" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -143,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -393,11 +410,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -405,7 +422,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,12 +443,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1173,6 +1193,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-582F-480F-982D-F342B035D432}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1833,60 +1858,65 @@
                   <c:v>7222.5815767565791</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>7216.0361222111242</c:v>
+                  <c:v>7229.1270313020341</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>7235.6724858474881</c:v>
+                  <c:v>7248.7633949383981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-582F-480F-982D-F342B035D432}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1980,7 +2010,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2009,7 +2038,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2751,6 +2780,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4EE-4274-B7CA-28DE6640CCAA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3465,6 +3499,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C4EE-4274-B7CA-28DE6640CCAA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3558,7 +3597,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3587,7 +3625,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3843,6 +3881,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E6D-4911-B7D4-713DCCB15B75}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4071,6 +4114,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1E6D-4911-B7D4-713DCCB15B75}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4164,7 +4212,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4193,7 +4240,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4935,6 +4982,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FB6-491A-A079-3CAEFC14C1BF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5595,7 +5647,7 @@
                   <c:v>5.6000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>-6.545454545454545</c:v>
+                  <c:v>6.545454545454545</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>19.636363636363633</c:v>
@@ -5649,6 +5701,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5FB6-491A-A079-3CAEFC14C1BF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5742,7 +5799,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5771,7 +5827,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6513,6 +6569,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B140-4A35-90E2-82355C117AB4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7227,6 +7288,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B140-4A35-90E2-82355C117AB4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7320,7 +7386,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7349,7 +7414,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7605,6 +7670,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26E7-406C-B085-D37879B65469}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7833,6 +7903,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-26E7-406C-B085-D37879B65469}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7926,7 +8001,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7971,7 +8045,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8001,7 +8081,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8033,7 +8119,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8065,7 +8157,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8097,7 +8195,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8129,7 +8233,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8150,9 +8260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8190,7 +8300,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -8262,7 +8372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8435,43 +8545,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1188" topLeftCell="A85" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1185" topLeftCell="A94" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="D5"/>
-      <selection pane="bottomLeft" activeCell="AL117" sqref="AL117"/>
+      <selection pane="bottomLeft" activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="6.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.33203125" style="2" customWidth="1"/>
-    <col min="8" max="10" width="6.77734375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="4.77734375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.77734375" style="6" customWidth="1"/>
-    <col min="15" max="16" width="6.77734375" style="2" customWidth="1"/>
-    <col min="17" max="18" width="4.77734375" style="6" customWidth="1"/>
-    <col min="19" max="20" width="8.33203125" style="2" customWidth="1"/>
-    <col min="21" max="23" width="6.77734375" style="2" customWidth="1"/>
-    <col min="24" max="25" width="4.77734375" style="6" customWidth="1"/>
-    <col min="26" max="26" width="6.77734375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="4.77734375" style="6" customWidth="1"/>
-    <col min="28" max="29" width="6.77734375" style="2" customWidth="1"/>
-    <col min="30" max="31" width="4.77734375" style="6" customWidth="1"/>
-    <col min="32" max="32" width="6.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="6.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.28515625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="6.7109375" style="2" customWidth="1"/>
+    <col min="11" max="12" width="4.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" style="6" customWidth="1"/>
+    <col min="15" max="16" width="6.7109375" style="2" customWidth="1"/>
+    <col min="17" max="18" width="4.7109375" style="6" customWidth="1"/>
+    <col min="19" max="20" width="8.28515625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="6.7109375" style="2" customWidth="1"/>
+    <col min="24" max="25" width="4.7109375" style="6" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" style="6" customWidth="1"/>
+    <col min="28" max="29" width="6.7109375" style="2" customWidth="1"/>
+    <col min="30" max="31" width="4.7109375" style="6" customWidth="1"/>
+    <col min="32" max="32" width="6.7109375" style="2" customWidth="1"/>
     <col min="33" max="33" width="11" style="2" customWidth="1"/>
-    <col min="34" max="34" width="6.77734375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="6.7109375" style="2" customWidth="1"/>
     <col min="35" max="35" width="11" style="2" customWidth="1"/>
-    <col min="36" max="36" width="6.77734375" style="2" customWidth="1"/>
+    <col min="36" max="36" width="6.7109375" style="2" customWidth="1"/>
     <col min="37" max="37" width="11" style="2" customWidth="1"/>
-    <col min="38" max="16384" width="8.88671875" style="2"/>
+    <col min="38" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -8485,7 +8595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8543,7 +8653,7 @@
       </c>
       <c r="AK2" s="27"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -8659,7 +8769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>42898</v>
       </c>
@@ -8783,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>42899</v>
       </c>
@@ -8907,7 +9017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>42900</v>
       </c>
@@ -9031,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>42901</v>
       </c>
@@ -9155,7 +9265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>42902</v>
       </c>
@@ -9279,7 +9389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>42903</v>
       </c>
@@ -9403,7 +9513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>42904</v>
       </c>
@@ -9527,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42905</v>
       </c>
@@ -9651,7 +9761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>42906</v>
       </c>
@@ -9775,7 +9885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>42907</v>
       </c>
@@ -9899,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>42908</v>
       </c>
@@ -10023,7 +10133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>42909</v>
       </c>
@@ -10147,7 +10257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>42910</v>
       </c>
@@ -10271,7 +10381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>42911</v>
       </c>
@@ -10395,7 +10505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>42912</v>
       </c>
@@ -10519,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>42913</v>
       </c>
@@ -10643,7 +10753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>42914</v>
       </c>
@@ -10770,7 +10880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>42915</v>
       </c>
@@ -10894,7 +11004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>42916</v>
       </c>
@@ -11018,7 +11128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>42917</v>
       </c>
@@ -11142,7 +11252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>42918</v>
       </c>
@@ -11266,7 +11376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>42919</v>
       </c>
@@ -11390,7 +11500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>42920</v>
       </c>
@@ -11514,7 +11624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>42921</v>
       </c>
@@ -11638,7 +11748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>42922</v>
       </c>
@@ -11765,7 +11875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>42923</v>
       </c>
@@ -11892,7 +12002,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>42924</v>
       </c>
@@ -12019,7 +12129,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>42925</v>
       </c>
@@ -12146,7 +12256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>42926</v>
       </c>
@@ -12273,7 +12383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>42927</v>
       </c>
@@ -12397,7 +12507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>42928</v>
       </c>
@@ -12521,7 +12631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>42929</v>
       </c>
@@ -12645,7 +12755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>42930</v>
       </c>
@@ -12769,7 +12879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>42931</v>
       </c>
@@ -12893,7 +13003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>42932</v>
       </c>
@@ -13017,7 +13127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>42933</v>
       </c>
@@ -13141,7 +13251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>42934</v>
       </c>
@@ -13265,7 +13375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>42935</v>
       </c>
@@ -13389,7 +13499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>42936</v>
       </c>
@@ -13513,7 +13623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42937</v>
       </c>
@@ -13637,7 +13747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42938</v>
       </c>
@@ -13761,7 +13871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42939</v>
       </c>
@@ -13885,7 +13995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>42940</v>
       </c>
@@ -14009,7 +14119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>42941</v>
       </c>
@@ -14133,7 +14243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>42942</v>
       </c>
@@ -14257,7 +14367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42943</v>
       </c>
@@ -14381,7 +14491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>42944</v>
       </c>
@@ -14505,7 +14615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>42945</v>
       </c>
@@ -14629,7 +14739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>42946</v>
       </c>
@@ -14753,7 +14863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>42947</v>
       </c>
@@ -14877,7 +14987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>42948</v>
       </c>
@@ -15001,7 +15111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>42949</v>
       </c>
@@ -15125,7 +15235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>42950</v>
       </c>
@@ -15249,7 +15359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>42951</v>
       </c>
@@ -15373,7 +15483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>42952</v>
       </c>
@@ -15497,7 +15607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>42953</v>
       </c>
@@ -15621,7 +15731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>42954</v>
       </c>
@@ -15745,7 +15855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>42955</v>
       </c>
@@ -15869,7 +15979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>42956</v>
       </c>
@@ -15993,7 +16103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>42957</v>
       </c>
@@ -16117,7 +16227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>42958</v>
       </c>
@@ -16241,7 +16351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>42959</v>
       </c>
@@ -16365,7 +16475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>42960</v>
       </c>
@@ -16489,7 +16599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>42961</v>
       </c>
@@ -16613,7 +16723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>42962</v>
       </c>
@@ -16737,7 +16847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>42963</v>
       </c>
@@ -16861,7 +16971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>42964</v>
       </c>
@@ -16985,7 +17095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>42965</v>
       </c>
@@ -17109,7 +17219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>42966</v>
       </c>
@@ -17233,7 +17343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>42967</v>
       </c>
@@ -17357,7 +17467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>42968</v>
       </c>
@@ -17481,7 +17591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>42969</v>
       </c>
@@ -17608,7 +17718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>42970</v>
       </c>
@@ -17735,7 +17845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>42971</v>
       </c>
@@ -17859,7 +17969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>42972</v>
       </c>
@@ -17983,7 +18093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>42973</v>
       </c>
@@ -18107,7 +18217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>42974</v>
       </c>
@@ -18231,7 +18341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>42975</v>
       </c>
@@ -18355,7 +18465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>42976</v>
       </c>
@@ -18482,7 +18592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>42977</v>
       </c>
@@ -18606,7 +18716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>42978</v>
       </c>
@@ -18730,7 +18840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>42979</v>
       </c>
@@ -18862,7 +18972,7 @@
         <v>78.545454545454547</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>42980</v>
       </c>
@@ -18994,7 +19104,7 @@
         <v>195.42424242424244</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>42981</v>
       </c>
@@ -19126,7 +19236,7 @@
         <v>397.24242424242425</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>42982</v>
       </c>
@@ -19258,7 +19368,7 @@
         <v>788.5151515151515</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>42983</v>
       </c>
@@ -19390,7 +19500,7 @@
         <v>982.219696969697</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>42984</v>
       </c>
@@ -19525,7 +19635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>42985</v>
       </c>
@@ -19660,7 +19770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>42986</v>
       </c>
@@ -19795,7 +19905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>42987</v>
       </c>
@@ -19927,7 +20037,7 @@
         <v>3528.9628787878783</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>42988</v>
       </c>
@@ -20059,7 +20169,7 @@
         <v>4830.9022727272722</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>42989</v>
       </c>
@@ -20191,7 +20301,7 @@
         <v>5435.9022727272722</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>42990</v>
       </c>
@@ -20323,7 +20433,7 @@
         <v>6113.4780303030302</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>42991</v>
       </c>
@@ -20455,7 +20565,7 @@
         <v>6481.7053030303032</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>42992</v>
       </c>
@@ -20590,7 +20700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>42993</v>
       </c>
@@ -20722,7 +20832,7 @@
         <v>8023.4992424242428</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>42994</v>
       </c>
@@ -20748,7 +20858,7 @@
         <v>46</v>
       </c>
       <c r="I100" s="7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J100" s="7">
         <v>0</v>
@@ -20791,7 +20901,7 @@
       </c>
       <c r="V100" s="10">
         <f t="shared" si="25"/>
-        <v>-6.545454545454545</v>
+        <v>6.545454545454545</v>
       </c>
       <c r="W100" s="10">
         <f t="shared" si="26"/>
@@ -20831,11 +20941,11 @@
       </c>
       <c r="AF100" s="28">
         <f t="shared" si="38"/>
-        <v>-6.545454545454545</v>
+        <v>6.545454545454545</v>
       </c>
       <c r="AG100" s="29">
         <f t="shared" si="37"/>
-        <v>7216.0361222111242</v>
+        <v>7229.1270313020341</v>
       </c>
       <c r="AH100" s="28">
         <f t="shared" si="39"/>
@@ -20857,7 +20967,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>42995</v>
       </c>
@@ -20970,7 +21080,7 @@
       </c>
       <c r="AG101" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH101" s="28">
         <f t="shared" si="39"/>
@@ -20989,7 +21099,7 @@
         <v>9087.117424242424</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>42996</v>
       </c>
@@ -21102,7 +21212,7 @@
       </c>
       <c r="AG102" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH102" s="28">
         <f t="shared" si="39"/>
@@ -21121,7 +21231,7 @@
         <v>9413.367424242424</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>42997</v>
       </c>
@@ -21234,7 +21344,7 @@
       </c>
       <c r="AG103" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH103" s="28">
         <f t="shared" si="39"/>
@@ -21253,7 +21363,7 @@
         <v>10722.458333333332</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>42998</v>
       </c>
@@ -21366,7 +21476,7 @@
       </c>
       <c r="AG104" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH104" s="28">
         <f t="shared" si="39"/>
@@ -21385,7 +21495,7 @@
         <v>11327.421969696969</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>42999</v>
       </c>
@@ -21498,7 +21608,7 @@
       </c>
       <c r="AG105" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH105" s="28">
         <f t="shared" si="39"/>
@@ -21520,7 +21630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>43000</v>
       </c>
@@ -21633,7 +21743,7 @@
       </c>
       <c r="AG106" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH106" s="28">
         <f t="shared" si="39"/>
@@ -21652,7 +21762,7 @@
         <v>12522.808333333332</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>43001</v>
       </c>
@@ -21765,7 +21875,7 @@
       </c>
       <c r="AG107" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH107" s="28">
         <f t="shared" si="39"/>
@@ -21784,7 +21894,7 @@
         <v>12941.717424242423</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>43002</v>
       </c>
@@ -21897,7 +22007,7 @@
       </c>
       <c r="AG108" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH108" s="28">
         <f t="shared" si="39"/>
@@ -21916,7 +22026,7 @@
         <v>13185.262878787877</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>43003</v>
       </c>
@@ -22029,7 +22139,7 @@
       </c>
       <c r="AG109" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH109" s="28">
         <f t="shared" si="39"/>
@@ -22051,7 +22161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>43004</v>
       </c>
@@ -22164,7 +22274,7 @@
       </c>
       <c r="AG110" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH110" s="28">
         <f t="shared" si="39"/>
@@ -22183,7 +22293,7 @@
         <v>13739.990151515149</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>43005</v>
       </c>
@@ -22296,7 +22406,7 @@
       </c>
       <c r="AG111" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH111" s="28">
         <f t="shared" si="39"/>
@@ -22318,7 +22428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>43006</v>
       </c>
@@ -22431,7 +22541,7 @@
       </c>
       <c r="AG112" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH112" s="28">
         <f t="shared" si="39"/>
@@ -22450,7 +22560,7 @@
         <v>14017.51742424242</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>43007</v>
       </c>
@@ -22563,7 +22673,7 @@
       </c>
       <c r="AG113" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH113" s="28">
         <f t="shared" si="39"/>
@@ -22582,7 +22692,7 @@
         <v>14217.578030303026</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>43008</v>
       </c>
@@ -22695,7 +22805,7 @@
       </c>
       <c r="AG114" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH114" s="28">
         <f t="shared" si="39"/>
@@ -22714,7 +22824,7 @@
         <v>14348.487121212116</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>43009</v>
       </c>
@@ -22827,7 +22937,7 @@
       </c>
       <c r="AG115" s="29">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH115" s="28">
         <f t="shared" si="39"/>
@@ -22849,7 +22959,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>43010</v>
       </c>
@@ -22962,7 +23072,7 @@
       </c>
       <c r="AG116" s="31">
         <f t="shared" si="37"/>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="AH116" s="30">
         <f t="shared" si="39"/>
@@ -22994,39 +23104,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R117"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="912" topLeftCell="A81" activePane="bottomLeft"/>
+      <pane ySplit="915" topLeftCell="A81" activePane="bottomLeft"/>
       <selection activeCell="X6" sqref="X6"/>
       <selection pane="bottomLeft" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2"/>
+    <col min="8" max="8" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="2"/>
-    <col min="14" max="14" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="2"/>
+    <col min="14" max="14" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="17" max="17" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -23037,7 +23147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
@@ -23087,7 +23197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>42898</v>
       </c>
@@ -23129,7 +23239,7 @@
         <v>8.2987041727114012E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>42899</v>
       </c>
@@ -23171,7 +23281,7 @@
         <v>1.5183555041923823E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>42900</v>
       </c>
@@ -23213,7 +23323,7 @@
         <v>2.0654552607637267E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>42901</v>
       </c>
@@ -23255,7 +23365,7 @@
         <v>3.0133516929356511E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <v>42902</v>
       </c>
@@ -23297,7 +23407,7 @@
         <v>4.2661486636012685E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>42903</v>
       </c>
@@ -23339,7 +23449,7 @@
         <v>5.3910841181243702E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>42904</v>
       </c>
@@ -23381,7 +23491,7 @@
         <v>6.6426516511347705E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>42905</v>
       </c>
@@ -23423,7 +23533,7 @@
         <v>8.2212496004327618E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>42906</v>
       </c>
@@ -23465,7 +23575,7 @@
         <v>0.1025842779512651</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <v>42907</v>
       </c>
@@ -23507,7 +23617,7 @@
         <v>0.1206938946126042</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>42908</v>
       </c>
@@ -23549,7 +23659,7 @@
         <v>0.14900784381224028</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>42909</v>
       </c>
@@ -23591,7 +23701,7 @@
         <v>0.18085027908234774</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>42910</v>
       </c>
@@ -23633,7 +23743,7 @@
         <v>0.20386535198800068</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <v>42911</v>
       </c>
@@ -23675,7 +23785,7 @@
         <v>0.23188423615038481</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <v>42912</v>
       </c>
@@ -23717,7 +23827,7 @@
         <v>0.25467801027809878</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>42913</v>
       </c>
@@ -23759,7 +23869,7 @@
         <v>0.28218053062529197</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <v>42914</v>
       </c>
@@ -23801,7 +23911,7 @@
         <v>0.31253534633258745</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <v>42915</v>
       </c>
@@ -23843,7 +23953,7 @@
         <v>0.34410730531854727</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <v>42916</v>
       </c>
@@ -23885,7 +23995,7 @@
         <v>0.37716688386731911</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <v>42917</v>
       </c>
@@ -23927,7 +24037,7 @@
         <v>0.40410386289311268</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>42918</v>
       </c>
@@ -23969,7 +24079,7 @@
         <v>0.43156950011064937</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <v>42919</v>
       </c>
@@ -24011,7 +24121,7 @@
         <v>0.4588261329267993</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="48">
         <v>42920</v>
       </c>
@@ -24053,7 +24163,7 @@
         <v>0.49934839804273523</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
         <v>42921</v>
       </c>
@@ -24095,7 +24205,7 @@
         <v>0.5290147286631095</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="48">
         <v>42922</v>
       </c>
@@ -24137,7 +24247,7 @@
         <v>0.56806166859278562</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="48">
         <v>42923</v>
       </c>
@@ -24179,7 +24289,7 @@
         <v>0.60446531756374633</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="48">
         <v>42924</v>
       </c>
@@ -24221,7 +24331,7 @@
         <v>0.62563623398657453</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="48">
         <v>42925</v>
       </c>
@@ -24263,7 +24373,7 @@
         <v>0.65478620079175787</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="48">
         <v>42926</v>
       </c>
@@ -24305,7 +24415,7 @@
         <v>0.67935036514298364</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="48">
         <v>42927</v>
       </c>
@@ -24347,7 +24457,7 @@
         <v>0.70650864294671623</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="48">
         <v>42928</v>
       </c>
@@ -24389,7 +24499,7 @@
         <v>0.73472423713393498</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="48">
         <v>42929</v>
       </c>
@@ -24431,7 +24541,7 @@
         <v>0.75980476530035157</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="48">
         <v>42930</v>
       </c>
@@ -24473,7 +24583,7 @@
         <v>0.78675403870269733</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="48">
         <v>42931</v>
       </c>
@@ -24515,7 +24625,7 @@
         <v>0.80837984705795574</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
         <v>42932</v>
       </c>
@@ -24557,7 +24667,7 @@
         <v>0.82566574049029973</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="48">
         <v>42933</v>
       </c>
@@ -24599,7 +24709,7 @@
         <v>0.84227544321227465</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
         <v>42934</v>
       </c>
@@ -24641,7 +24751,7 @@
         <v>0.85661068627209913</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="48">
         <v>42935</v>
       </c>
@@ -24683,7 +24793,7 @@
         <v>0.86869605842287734</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
         <v>42936</v>
       </c>
@@ -24725,7 +24835,7 @@
         <v>0.87912168973911331</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <v>42937</v>
       </c>
@@ -24767,7 +24877,7 @@
         <v>0.8897809142098404</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="48">
         <v>42938</v>
       </c>
@@ -24809,7 +24919,7 @@
         <v>0.89986230298261571</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="48">
         <v>42939</v>
       </c>
@@ -24851,7 +24961,7 @@
         <v>0.90789053087117955</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="48">
         <v>42940</v>
       </c>
@@ -24893,7 +25003,7 @@
         <v>0.91810715778602869</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="48">
         <v>42941</v>
       </c>
@@ -24935,7 +25045,7 @@
         <v>0.92650421697115737</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="48">
         <v>42942</v>
       </c>
@@ -24977,7 +25087,7 @@
         <v>0.93520863557009026</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
         <v>42943</v>
       </c>
@@ -25019,7 +25129,7 @@
         <v>0.94343357348348866</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
         <v>42944</v>
       </c>
@@ -25061,7 +25171,7 @@
         <v>0.94996188743268828</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="48">
         <v>42945</v>
       </c>
@@ -25103,7 +25213,7 @@
         <v>0.95464604489906313</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="48">
         <v>42946</v>
       </c>
@@ -25145,7 +25255,7 @@
         <v>0.95999409869925501</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
         <v>42947</v>
       </c>
@@ -25187,7 +25297,7 @@
         <v>0.96365782291180013</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
         <v>42948</v>
       </c>
@@ -25229,7 +25339,7 @@
         <v>0.96687894956846743</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
         <v>42949</v>
       </c>
@@ -25271,7 +25381,7 @@
         <v>0.96973124492856966</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
         <v>42950</v>
       </c>
@@ -25313,7 +25423,7 @@
         <v>0.97265730654798499</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
         <v>42951</v>
       </c>
@@ -25355,7 +25465,7 @@
         <v>0.97650544640881265</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
         <v>42952</v>
       </c>
@@ -25397,7 +25507,7 @@
         <v>0.97976345619513638</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
         <v>42953</v>
       </c>
@@ -25439,7 +25549,7 @@
         <v>0.98260345717868647</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
         <v>42954</v>
       </c>
@@ -25481,7 +25591,7 @@
         <v>0.98533280877326712</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
         <v>42955</v>
       </c>
@@ -25523,7 +25633,7 @@
         <v>0.98683272271263123</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
         <v>42956</v>
       </c>
@@ -25565,7 +25675,7 @@
         <v>0.98829575352233889</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="48">
         <v>42957</v>
       </c>
@@ -25607,7 +25717,7 @@
         <v>0.99012761562861151</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="48">
         <v>42958</v>
       </c>
@@ -25649,7 +25759,7 @@
         <v>0.99138164203693235</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="48">
         <v>42959</v>
       </c>
@@ -25691,7 +25801,7 @@
         <v>0.99263566844525319</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="48">
         <v>42960</v>
       </c>
@@ -25733,7 +25843,7 @@
         <v>0.9940864048784086</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="48">
         <v>42961</v>
       </c>
@@ -25775,7 +25885,7 @@
         <v>0.99535272566328159</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="48">
         <v>42962</v>
       </c>
@@ -25817,7 +25927,7 @@
         <v>0.99604121075020291</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="48">
         <v>42963</v>
       </c>
@@ -25859,7 +25969,7 @@
         <v>0.99671740146057197</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="48">
         <v>42964</v>
       </c>
@@ -25901,7 +26011,7 @@
         <v>0.99709852713368907</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="48">
         <v>42965</v>
       </c>
@@ -25943,7 +26053,7 @@
         <v>0.99743047530059747</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="48">
         <v>42966</v>
       </c>
@@ -25985,7 +26095,7 @@
         <v>0.99792225036268412</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="48">
         <v>42967</v>
       </c>
@@ -26027,7 +26137,7 @@
         <v>0.99827878728269692</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="48">
         <v>42968</v>
       </c>
@@ -26069,7 +26179,7 @@
         <v>0.99868450170891832</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="48">
         <v>42969</v>
       </c>
@@ -26111,7 +26221,7 @@
         <v>0.99889350611030514</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="48">
         <v>42970</v>
       </c>
@@ -26153,7 +26263,7 @@
         <v>0.99911480488824411</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="48">
         <v>42971</v>
       </c>
@@ -26195,7 +26305,7 @@
         <v>0.9992131599006614</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="48">
         <v>42972</v>
       </c>
@@ -26237,7 +26347,7 @@
         <v>0.99927463178342224</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="48">
         <v>42973</v>
       </c>
@@ -26279,7 +26389,7 @@
         <v>0.99942216430204822</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="48">
         <v>42974</v>
       </c>
@@ -26321,7 +26431,7 @@
         <v>0.99959428557377861</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="48">
         <v>42975</v>
       </c>
@@ -26363,7 +26473,7 @@
         <v>0.99969264058619589</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="48">
         <v>42976</v>
       </c>
@@ -26405,7 +26515,7 @@
         <v>0.99972952371585233</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="48">
         <v>42977</v>
       </c>
@@ -26447,7 +26557,7 @@
         <v>0.99979099559861317</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="48">
         <v>42978</v>
       </c>
@@ -26489,7 +26599,7 @@
         <v>0.99985246748137402</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="48">
         <v>42979</v>
       </c>
@@ -26549,7 +26659,7 @@
         <v>1.4730771641697487E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="48">
         <v>42980</v>
       </c>
@@ -26609,7 +26719,7 @@
         <v>3.3285275496771766E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="48">
         <v>42981</v>
       </c>
@@ -26669,7 +26779,7 @@
         <v>5.5976932238450447E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="48">
         <v>42982</v>
       </c>
@@ -26729,7 +26839,7 @@
         <v>8.1677427443114153E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="48">
         <v>42983</v>
       </c>
@@ -26789,7 +26899,7 @@
         <v>0.11126433899580017</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="48">
         <v>42984</v>
       </c>
@@ -26849,7 +26959,7 @@
         <v>0.1441735096846988</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="48">
         <v>42985</v>
       </c>
@@ -26909,7 +27019,7 @@
         <v>0.17156647652479157</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="48">
         <v>42986</v>
       </c>
@@ -26969,7 +27079,7 @@
         <v>0.20497712029085438</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="48">
         <v>42987</v>
       </c>
@@ -27029,7 +27139,7 @@
         <v>0.2363818717482605</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="48">
         <v>42988</v>
       </c>
@@ -27089,7 +27199,7 @@
         <v>0.27286403811195387</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="48">
         <v>42989</v>
       </c>
@@ -27149,7 +27259,7 @@
         <v>0.33109759919764309</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="48">
         <v>42990</v>
       </c>
@@ -27209,7 +27319,7 @@
         <v>0.36971102613928414</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="48">
         <v>42991</v>
       </c>
@@ -27269,7 +27379,7 @@
         <v>0.40443803673290291</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="48">
         <v>42992</v>
       </c>
@@ -27329,7 +27439,7 @@
         <v>0.43621889299818217</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="48">
         <v>42993</v>
       </c>
@@ -27389,7 +27499,7 @@
         <v>0.47746505359493513</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="48">
         <v>42994</v>
       </c>
@@ -27401,11 +27511,11 @@
       </c>
       <c r="D99" s="4">
         <f>Counts!AF100</f>
-        <v>-6.545454545454545</v>
+        <v>6.545454545454545</v>
       </c>
       <c r="E99" s="4">
         <f>Counts!AG100</f>
-        <v>7216.0361222111242</v>
+        <v>7229.1270313020341</v>
       </c>
       <c r="F99" s="50">
         <f t="shared" si="2"/>
@@ -27449,7 +27559,7 @@
         <v>0.52698551996489684</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="48">
         <v>42995</v>
       </c>
@@ -27465,7 +27575,7 @@
       </c>
       <c r="E100" s="4">
         <f>Counts!AG101</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F100" s="50">
         <f t="shared" si="2"/>
@@ -27509,7 +27619,7 @@
         <v>0.56290352911678054</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="48">
         <v>42996</v>
       </c>
@@ -27525,7 +27635,7 @@
       </c>
       <c r="E101" s="4">
         <f>Counts!AG102</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F101" s="50">
         <f t="shared" si="2"/>
@@ -27569,7 +27679,7 @@
         <v>0.60233184980881338</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="48">
         <v>42997</v>
       </c>
@@ -27585,7 +27695,7 @@
       </c>
       <c r="E102" s="4">
         <f>Counts!AG103</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F102" s="50">
         <f t="shared" si="2"/>
@@ -27629,7 +27739,7 @@
         <v>0.64558390271422306</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="48">
         <v>42998</v>
       </c>
@@ -27645,7 +27755,7 @@
       </c>
       <c r="E103" s="4">
         <f>Counts!AG104</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F103" s="50">
         <f t="shared" si="2"/>
@@ -27689,7 +27799,7 @@
         <v>0.67698865417162912</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="48">
         <v>42999</v>
       </c>
@@ -27705,7 +27815,7 @@
       </c>
       <c r="E104" s="4">
         <f>Counts!AG105</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F104" s="50">
         <f t="shared" si="2"/>
@@ -27749,7 +27859,7 @@
         <v>0.70745314360935252</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="48">
         <v>43000</v>
       </c>
@@ -27765,7 +27875,7 @@
       </c>
       <c r="E105" s="4">
         <f>Counts!AG106</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F105" s="50">
         <f t="shared" si="2"/>
@@ -27809,7 +27919,7 @@
         <v>0.74186673352974364</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="48">
         <v>43001</v>
       </c>
@@ -27825,7 +27935,7 @@
       </c>
       <c r="E106" s="4">
         <f>Counts!AG107</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F106" s="50">
         <f t="shared" si="2"/>
@@ -27869,7 +27979,7 @@
         <v>0.7742117470068326</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="48">
         <v>43002</v>
       </c>
@@ -27885,7 +27995,7 @@
       </c>
       <c r="E107" s="4">
         <f>Counts!AG108</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F107" s="50">
         <f t="shared" si="2"/>
@@ -27929,7 +28039,7 @@
         <v>0.8154579076035855</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="48">
         <v>43003</v>
       </c>
@@ -27945,7 +28055,7 @@
       </c>
       <c r="E108" s="4">
         <f>Counts!AG109</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F108" s="50">
         <f t="shared" si="2"/>
@@ -27989,7 +28099,7 @@
         <v>0.84416724127123421</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="48">
         <v>43004</v>
       </c>
@@ -28005,7 +28115,7 @@
       </c>
       <c r="E109" s="4">
         <f>Counts!AG110</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F109" s="50">
         <f t="shared" si="2"/>
@@ -28049,7 +28159,7 @@
         <v>0.87112141916880836</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="48">
         <v>43005</v>
       </c>
@@ -28065,7 +28175,7 @@
       </c>
       <c r="E110" s="4">
         <f>Counts!AG111</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F110" s="50">
         <f t="shared" si="2"/>
@@ -28109,7 +28219,7 @@
         <v>0.90171127687582275</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="48">
         <v>43006</v>
       </c>
@@ -28125,7 +28235,7 @@
       </c>
       <c r="E111" s="4">
         <f>Counts!AG112</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F111" s="50">
         <f t="shared" si="2"/>
@@ -28169,7 +28279,7 @@
         <v>0.91988967592302384</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="48">
         <v>43007</v>
       </c>
@@ -28185,7 +28295,7 @@
       </c>
       <c r="E112" s="4">
         <f>Counts!AG113</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F112" s="50">
         <f t="shared" si="2"/>
@@ -28229,7 +28339,7 @@
         <v>0.94684385382059799</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="48">
         <v>43008</v>
       </c>
@@ -28245,7 +28355,7 @@
       </c>
       <c r="E113" s="4">
         <f>Counts!AG114</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F113" s="50">
         <f t="shared" si="2"/>
@@ -28289,7 +28399,7 @@
         <v>0.96815645960007524</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="48">
         <v>43009</v>
       </c>
@@ -28305,7 +28415,7 @@
       </c>
       <c r="E114" s="4">
         <f>Counts!AG115</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F114" s="50">
         <f t="shared" si="2"/>
@@ -28349,7 +28459,7 @@
         <v>0.9883407509559331</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="48">
         <v>43010</v>
       </c>
@@ -28365,7 +28475,7 @@
       </c>
       <c r="E115" s="4">
         <f>Counts!AG116</f>
-        <v>7235.6724858474881</v>
+        <v>7248.7633949383981</v>
       </c>
       <c r="F115" s="50">
         <f t="shared" si="2"/>
@@ -28409,10 +28519,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="49"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="49"/>
     </row>
   </sheetData>

</xml_diff>